<commit_message>
added all packages and classes
</commit_message>
<xml_diff>
--- a/Pizza-delievry-system/target/classes/Team 4 rest-services.xlsx
+++ b/Pizza-delievry-system/target/classes/Team 4 rest-services.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRIYAMVAD\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27519E1B-A23D-46CD-925D-3846496296CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C105AAEC-FAD9-4473-9EFD-7AD12EE8F7BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{420ED039-64A4-44EE-925E-22693EDBA285}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="136">
   <si>
     <t xml:space="preserve"> FOOD rest services   </t>
   </si>
@@ -252,19 +252,10 @@
 of user </t>
   </si>
   <si>
-    <t>/card</t>
-  </si>
-  <si>
     <t>POST</t>
   </si>
   <si>
-    <t>/verifycard</t>
-  </si>
-  <si>
     <t>DELETE</t>
-  </si>
-  <si>
-    <t>/order</t>
   </si>
   <si>
     <t>/food</t>
@@ -296,12 +287,6 @@
   </si>
   <si>
     <t>?search=string to be searched</t>
-  </si>
-  <si>
-    <t>/sortbyprice</t>
-  </si>
-  <si>
-    <t>/searchfood</t>
   </si>
   <si>
     <t>?foodtype=type of food</t>
@@ -387,9 +372,6 @@
 ]</t>
   </si>
   <si>
-    <t>/foodbytype</t>
-  </si>
-  <si>
     <t xml:space="preserve"> get all store where a particular food is present</t>
   </si>
   <si>
@@ -420,16 +402,6 @@
 </t>
   </si>
   <si>
-    <t>/login</t>
-  </si>
-  <si>
-    <t>/logout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/register
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">authKey=
 sessionId of 
 user </t>
@@ -451,9 +423,6 @@
 }</t>
   </si>
   <si>
-    <t>/profile</t>
-  </si>
-  <si>
     <t>get all credit card details</t>
   </si>
   <si>
@@ -487,9 +456,6 @@
  }</t>
   </si>
   <si>
-    <t>/changepassword</t>
-  </si>
-  <si>
     <t>{
  UserId:"1001",
 Fistname:"first name",
@@ -506,9 +472,6 @@
 }</t>
   </si>
   <si>
-    <t>/profileupdate</t>
-  </si>
-  <si>
     <t>{
  Cost:"Total Cost"
 FoodId:"10001",
@@ -516,9 +479,6 @@
 Quantity:"quantity of pizza",
 OrdateDate:"YYYY-DD-MM"
 }</t>
-  </si>
-  <si>
-    <t>/cart</t>
   </si>
   <si>
     <t>?id=cart unique id</t>
@@ -616,19 +576,10 @@
 </t>
   </si>
   <si>
-    <t>/orderbydate</t>
-  </si>
-  <si>
-    <t>/orderbystatus</t>
-  </si>
-  <si>
     <t xml:space="preserve">?status= confirmed || delievered 
  || pending ||cancelled
  in plain string
 </t>
-  </si>
-  <si>
-    <t>/updatestore</t>
   </si>
   <si>
     <t>{
@@ -665,12 +616,6 @@
  }
 ]
 </t>
-  </si>
-  <si>
-    <t>/storebyfood</t>
-  </si>
-  <si>
-    <t>/foodbystore</t>
   </si>
   <si>
     <t>get all cart details</t>
@@ -747,6 +692,106 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>/food/sort/price</t>
+  </si>
+  <si>
+    <t>/food/search</t>
+  </si>
+  <si>
+    <t>/food/type</t>
+  </si>
+  <si>
+    <t>/store/food</t>
+  </si>
+  <si>
+    <t>/store/food/{id}</t>
+  </si>
+  <si>
+    <t>{StoreId:101
+ Name:"StoreName"
+ Street:"Store Street"
+ MobileNo:"99xxxxxxxx"
+ City:"StoreCity"
+ State:"StoreState"
+ Pincode:"Store Pincode"
+ }</t>
+  </si>
+  <si>
+    <t>/user/login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/user
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{UserID:101
+ "FirstName": "somename"
+ "LastName": "somename"
+ "DateOfBirth": "date"
+ "Gender": "gender"
+ "Street": "streetname"
+ "Location": "landmark"
+ "City": "cityname"
+ "State": "statename"
+ "Pincode": "pin" 
+ "MobileNo": 9xxxxxxxx
+ "EmailId": "abc@xyz.com"
+"Password":"password"
+}
+</t>
+  </si>
+  <si>
+    <t>/user/logout</t>
+  </si>
+  <si>
+    <t>/user/profile</t>
+  </si>
+  <si>
+    <t>/user/changepassword</t>
+  </si>
+  <si>
+    <t>/user</t>
+  </si>
+  <si>
+    <t>/user/cart/item</t>
+  </si>
+  <si>
+    <t>/food/order</t>
+  </si>
+  <si>
+    <t>{OrderId:101
+OrderDate:"YYYY-DD-MM"
+StoreId:"storeId"
+OrderStatus:"Confirmed"
+cartid:"id of cart"
+Street: "streetname"
+Location: "landmark"
+City: "cityname"
+State: "statename"
+PinCode:"pncode"
+mobile number:"99xxxxxxxx"
+totalprice:1500
+}</t>
+  </si>
+  <si>
+    <t>/user/order</t>
+  </si>
+  <si>
+    <t>/user/order/filter/date</t>
+  </si>
+  <si>
+    <t>/user/order/filter/status</t>
+  </si>
+  <si>
+    <t>/user/creditcard</t>
+  </si>
+  <si>
+    <t>/user/creditcard/verify</t>
+  </si>
+  <si>
+    <t>/user/cart</t>
   </si>
 </sst>
 </file>
@@ -1124,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5257770C-153E-4746-BFF5-05EBB845E977}">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,13 +1227,13 @@
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K4" t="s">
         <v>52</v>
@@ -1199,7 +1244,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1208,13 +1253,13 @@
         <v>62</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K5" t="s">
         <v>52</v>
@@ -1225,7 +1270,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1234,10 +1279,10 @@
         <v>62</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>61</v>
@@ -1251,7 +1296,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -1260,13 +1305,13 @@
         <v>62</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K7" t="s">
         <v>52</v>
@@ -1280,13 +1325,13 @@
         <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K8" t="s">
         <v>53</v>
@@ -1297,19 +1342,19 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G9" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="H9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K9" t="s">
         <v>53</v>
@@ -1320,19 +1365,19 @@
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G10" t="s">
-        <v>85</v>
+        <v>116</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K10" t="s">
         <v>53</v>
@@ -1361,22 +1406,22 @@
     </row>
     <row r="14" spans="1:11" ht="315" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="G14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K14" t="s">
         <v>54</v>
@@ -1387,19 +1432,19 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K15" t="s">
         <v>54</v>
@@ -1410,7 +1455,7 @@
         <v>19</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -1419,13 +1464,13 @@
         <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="G16" t="s">
         <v>63</v>
       </c>
       <c r="H16" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K16" t="s">
         <v>54</v>
@@ -1445,13 +1490,13 @@
         <v>62</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G17" t="s">
         <v>63</v>
       </c>
       <c r="H17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K17" t="s">
         <v>54</v>
@@ -1468,10 +1513,10 @@
         <v>7</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="H18" t="s">
         <v>61</v>
@@ -1490,7 +1535,7 @@
         <v>24</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
         <v>16</v>
@@ -1499,13 +1544,13 @@
         <v>25</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G22" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="H22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K22" t="s">
         <v>56</v>
@@ -1516,19 +1561,19 @@
         <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>56</v>
@@ -1539,16 +1584,16 @@
         <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G24" t="s">
-        <v>91</v>
+        <v>123</v>
       </c>
       <c r="H24" t="s">
         <v>68</v>
@@ -1562,19 +1607,19 @@
         <v>28</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G25" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="H25" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K25" t="s">
         <v>56</v>
@@ -1585,19 +1630,19 @@
         <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
         <v>30</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G26" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="H26" t="s">
         <v>61</v>
@@ -1611,19 +1656,19 @@
         <v>31</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>61</v>
@@ -1637,22 +1682,22 @@
         <v>32</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
         <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K28" t="s">
         <v>55</v>
@@ -1663,22 +1708,22 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="D29" t="s">
         <v>30</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G29" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="H29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K29" t="s">
         <v>55</v>
@@ -1689,22 +1734,22 @@
         <v>34</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D30" t="s">
         <v>30</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>71</v>
+        <v>128</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K30" t="s">
         <v>57</v>
@@ -1718,16 +1763,16 @@
         <v>30</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>71</v>
+        <v>130</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K31" t="s">
         <v>57</v>
@@ -1738,22 +1783,22 @@
         <v>36</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="D32" t="s">
         <v>30</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K32" t="s">
         <v>57</v>
@@ -1764,22 +1809,22 @@
         <v>37</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D33" t="s">
         <v>30</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K33" t="s">
         <v>57</v>
@@ -1799,24 +1844,24 @@
         <v>65</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="K34" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
         <v>30</v>
@@ -1825,13 +1870,13 @@
         <v>65</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>108</v>
+        <v>64</v>
       </c>
       <c r="G35" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="H35" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K35" t="s">
         <v>58</v>
@@ -1842,7 +1887,7 @@
         <v>48</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="D36" t="s">
         <v>30</v>
@@ -1851,13 +1896,13 @@
         <v>66</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G36" t="s">
-        <v>67</v>
+        <v>133</v>
       </c>
       <c r="H36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K36" t="s">
         <v>58</v>
@@ -1865,22 +1910,22 @@
     </row>
     <row r="37" spans="1:11" ht="345" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="G37" t="s">
-        <v>67</v>
+        <v>133</v>
       </c>
       <c r="H37" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K37" t="s">
         <v>58</v>
@@ -1888,19 +1933,19 @@
     </row>
     <row r="38" spans="1:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="G38" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="H38" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K38" t="s">
         <v>58</v>
@@ -1908,10 +1953,10 @@
     </row>
     <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="D39" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>66</v>
@@ -1919,36 +1964,48 @@
     </row>
     <row r="40" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D40" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D41" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>108</v>
+        <v>95</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -1990,7 +2047,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B54" t="s">
         <v>42</v>
@@ -1998,10 +2055,10 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="B55" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>